<commit_message>
functionality split into lifecycle and security pages
</commit_message>
<xml_diff>
--- a/output/FirstToGiven.xlsx
+++ b/output/FirstToGiven.xlsx
@@ -29,7 +29,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.10</t>
+    <t>0.4.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -50,7 +50,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-28T23:23:22-07:00</t>
+    <t>2022-09-29T00:03:59-07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>